<commit_message>
add top 10 columns filter
</commit_message>
<xml_diff>
--- a/03. Planilhas/Feature Selection.xlsx
+++ b/03. Planilhas/Feature Selection.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Feature Selection" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="113">
   <si>
     <t>data_obito</t>
   </si>
@@ -355,6 +355,9 @@
   </si>
   <si>
     <t>FS_U</t>
+  </si>
+  <si>
+    <t>Top 10 ambos</t>
   </si>
 </sst>
 </file>
@@ -1188,10 +1191,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H109"/>
+  <dimension ref="A1:K109"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1202,10 +1205,13 @@
     <col min="4" max="5" width="8.88671875" style="1"/>
     <col min="6" max="6" width="3.33203125" style="1" customWidth="1"/>
     <col min="7" max="8" width="23.44140625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="1"/>
+    <col min="9" max="9" width="3.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>109</v>
       </c>
@@ -1224,8 +1230,14 @@
       <c r="H1" s="3" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1246,8 +1258,15 @@
         <f>INDEX($B$2:$B$109,MATCH(E2,$A$2:$A$109,0),1)</f>
         <v>data_nasc</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J2" s="1">
+        <f>INDEX($A$2:$A$109,MATCH(K2,$B$2:$B$109,0),1)</f>
+        <v>2</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f>A2+1</f>
         <v>1</v>
@@ -1269,10 +1288,17 @@
         <f t="shared" ref="H3:H66" si="1">INDEX($B$2:$B$109,MATCH(E3,$A$2:$A$109,0),1)</f>
         <v>data_obito</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J3" s="1">
+        <f t="shared" ref="J3:J19" si="2">INDEX($A$2:$A$109,MATCH(K3,$B$2:$B$109,0),1)</f>
+        <v>4</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <f t="shared" ref="A4:A67" si="2">A3+1</f>
+        <f t="shared" ref="A4:A67" si="3">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1292,102 +1318,137 @@
         <f t="shared" si="1"/>
         <v>def_raca_cor_indÃ­gena</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J4" s="1">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>27</v>
+      </c>
+      <c r="G5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>data_obito</v>
+      </c>
+      <c r="H5" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>def_sexo_ignorado</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1">
+        <v>85</v>
+      </c>
+      <c r="G6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>idade_obito</v>
+      </c>
+      <c r="H6" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>res_rsaudcod_3517</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3</v>
+      </c>
+      <c r="E7" s="1">
+        <v>79</v>
+      </c>
+      <c r="G7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>idade_obito_calculado</v>
+      </c>
+      <c r="H7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>res_rsaudcod_3511</v>
+      </c>
+      <c r="J7" s="1">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1">
-        <v>27</v>
-      </c>
-      <c r="G5" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>data_obito</v>
-      </c>
-      <c r="H5" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>def_sexo_ignorado</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="1">
-        <v>11</v>
-      </c>
-      <c r="E6" s="1">
-        <v>85</v>
-      </c>
-      <c r="G6" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>idade_obito</v>
-      </c>
-      <c r="H6" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>res_rsaudcod_3517</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="1">
+        <v>5</v>
+      </c>
+      <c r="E8" s="1">
+        <v>24</v>
+      </c>
+      <c r="G8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>idade_obito_anos</v>
+      </c>
+      <c r="H8" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>dia_semana_nasc_sex</v>
+      </c>
+      <c r="J8" s="1">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="1">
-        <v>3</v>
-      </c>
-      <c r="E7" s="1">
-        <v>79</v>
-      </c>
-      <c r="G7" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>idade_obito_calculado</v>
-      </c>
-      <c r="H7" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>res_rsaudcod_3511</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="1">
-        <v>5</v>
-      </c>
-      <c r="E8" s="1">
-        <v>24</v>
-      </c>
-      <c r="G8" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>idade_obito_anos</v>
-      </c>
-      <c r="H8" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>dia_semana_nasc_sex</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1407,10 +1468,17 @@
         <f t="shared" si="1"/>
         <v>dia_semana_obito_qui</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J9" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1430,10 +1498,17 @@
         <f t="shared" si="1"/>
         <v>dia_semana_obito_qua</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J10" s="1">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1453,10 +1528,17 @@
         <f t="shared" si="1"/>
         <v>dia_semana_obito_sab</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J11" s="1">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1476,10 +1558,17 @@
         <f t="shared" si="1"/>
         <v>dia_semana_obito_ter</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J12" s="1">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1499,10 +1588,17 @@
         <f t="shared" si="1"/>
         <v>dia_semana_nasc_ter</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J13" s="1">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1522,125 +1618,167 @@
         <f t="shared" si="1"/>
         <v>dia_semana_obito_seg</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J14" s="1">
+        <f t="shared" si="2"/>
+        <v>85</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="1">
+        <v>58</v>
+      </c>
+      <c r="E15" s="1">
+        <v>21</v>
+      </c>
+      <c r="G15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>def_cirurgia_ignorado</v>
+      </c>
+      <c r="H15" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>dia_semana_nasc_qui</v>
+      </c>
+      <c r="J15" s="1">
+        <f t="shared" si="2"/>
+        <v>79</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="1">
+        <v>35</v>
+      </c>
+      <c r="E16" s="1">
+        <v>34</v>
+      </c>
+      <c r="G16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>def_est_civil_casado</v>
+      </c>
+      <c r="H16" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>def_raca_cor_preta</v>
+      </c>
+      <c r="J16" s="1">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="1">
+        <v>47</v>
+      </c>
+      <c r="E17" s="1">
+        <v>17</v>
+      </c>
+      <c r="G17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>def_loc_ocor_hospital</v>
+      </c>
+      <c r="H17" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>dia_semana_obito_sex</v>
+      </c>
+      <c r="J17" s="1">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="1">
+        <v>36</v>
+      </c>
+      <c r="E18" s="1">
+        <v>22</v>
+      </c>
+      <c r="G18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>def_est_civil_ignorado</v>
+      </c>
+      <c r="H18" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>dia_semana_nasc_sab</v>
+      </c>
+      <c r="J18" s="1">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="1">
-        <v>58</v>
-      </c>
-      <c r="E15" s="1">
-        <v>21</v>
-      </c>
-      <c r="G15" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>def_cirurgia_ignorado</v>
-      </c>
-      <c r="H15" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>dia_semana_nasc_qui</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <f t="shared" si="2"/>
-        <v>14</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="1">
-        <v>35</v>
-      </c>
-      <c r="E16" s="1">
-        <v>34</v>
-      </c>
-      <c r="G16" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>def_est_civil_casado</v>
-      </c>
-      <c r="H16" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>def_raca_cor_preta</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="1">
+        <v>95</v>
+      </c>
+      <c r="E19" s="1">
+        <v>72</v>
+      </c>
+      <c r="G19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>grande_grupo_ocup_forÃ§as_armadas_policiais_e_bombeiros_militares</v>
+      </c>
+      <c r="H19" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>res_rsaudcod_3504</v>
+      </c>
+      <c r="J19" s="1">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="1">
-        <v>47</v>
-      </c>
-      <c r="E17" s="1">
-        <v>17</v>
-      </c>
-      <c r="G17" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>def_loc_ocor_hospital</v>
-      </c>
-      <c r="H17" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>dia_semana_obito_sex</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="1">
-        <v>36</v>
-      </c>
-      <c r="E18" s="1">
-        <v>22</v>
-      </c>
-      <c r="G18" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>def_est_civil_ignorado</v>
-      </c>
-      <c r="H18" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>dia_semana_nasc_sab</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <f t="shared" si="2"/>
-        <v>17</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="1">
-        <v>95</v>
-      </c>
-      <c r="E19" s="1">
-        <v>72</v>
-      </c>
-      <c r="G19" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>grande_grupo_ocup_forÃ§as_armadas_policiais_e_bombeiros_militares</v>
-      </c>
-      <c r="H19" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>res_rsaudcod_3504</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1660,10 +1798,11 @@
         <f t="shared" si="1"/>
         <v>def_raca_cor_amarela</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J20"/>
+    </row>
+    <row r="21" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1683,10 +1822,11 @@
         <f t="shared" si="1"/>
         <v>res_rsaudcod_3509</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J21"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -1707,9 +1847,9 @@
         <v>def_loc_ocor_ignorado</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1730,9 +1870,9 @@
         <v>res_rsaudcod_3513</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -1753,9 +1893,9 @@
         <v>dia_semana_nasc_seg</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -1776,9 +1916,9 @@
         <v>dia_semana_obito_dom</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -1799,9 +1939,9 @@
         <v>res_rsaudcod_3508</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -1822,9 +1962,9 @@
         <v>dia_semana_nasc_qua</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -1845,9 +1985,9 @@
         <v>dia_semana_nasc_dom</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -1868,9 +2008,9 @@
         <v>res_rsaudcod_3507</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -1891,9 +2031,9 @@
         <v>def_loc_ocor_outros</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -1914,9 +2054,9 @@
         <v>res_rsaudcod_3520</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -1939,7 +2079,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1962,7 +2102,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -1985,7 +2125,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -2008,7 +2148,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -2031,7 +2171,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -2054,7 +2194,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -2077,7 +2217,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>37</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -2100,7 +2240,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -2123,7 +2263,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>39</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -2146,7 +2286,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -2169,7 +2309,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>41</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -2192,7 +2332,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>42</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -2215,7 +2355,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -2238,7 +2378,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>44</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -2261,7 +2401,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -2284,7 +2424,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>46</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -2307,7 +2447,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>47</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -2330,7 +2470,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>48</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -2353,7 +2493,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>49</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -2376,7 +2516,7 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -2399,7 +2539,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>51</v>
       </c>
       <c r="B53" s="1" t="s">
@@ -2422,7 +2562,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>52</v>
       </c>
       <c r="B54" s="1" t="s">
@@ -2445,7 +2585,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>53</v>
       </c>
       <c r="B55" s="1" t="s">
@@ -2468,7 +2608,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>54</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -2491,7 +2631,7 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>55</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -2514,7 +2654,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>56</v>
       </c>
       <c r="B58" s="1" t="s">
@@ -2537,7 +2677,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>57</v>
       </c>
       <c r="B59" s="1" t="s">
@@ -2560,7 +2700,7 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>58</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -2583,7 +2723,7 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>59</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -2606,7 +2746,7 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="B62" s="1" t="s">
@@ -2629,7 +2769,7 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>61</v>
       </c>
       <c r="B63" s="1" t="s">
@@ -2652,7 +2792,7 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>62</v>
       </c>
       <c r="B64" s="1" t="s">
@@ -2675,7 +2815,7 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>63</v>
       </c>
       <c r="B65" s="1" t="s">
@@ -2698,7 +2838,7 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>64</v>
       </c>
       <c r="B66" s="1" t="s">
@@ -2721,7 +2861,7 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>65</v>
       </c>
       <c r="B67" s="1" t="s">
@@ -2734,17 +2874,17 @@
         <v>28</v>
       </c>
       <c r="G67" s="1" t="str">
-        <f t="shared" ref="G67:G109" si="3">INDEX($B$2:$B$109,MATCH(D67,$A$2:$A$109,0),1)</f>
+        <f t="shared" ref="G67:G109" si="4">INDEX($B$2:$B$109,MATCH(D67,$A$2:$A$109,0),1)</f>
         <v>res_longitude</v>
       </c>
       <c r="H67" s="1" t="str">
-        <f t="shared" ref="H67:H109" si="4">INDEX($B$2:$B$109,MATCH(E67,$A$2:$A$109,0),1)</f>
+        <f t="shared" ref="H67:H109" si="5">INDEX($B$2:$B$109,MATCH(E67,$A$2:$A$109,0),1)</f>
         <v>def_sexo_masculino</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <f t="shared" ref="A68:A109" si="5">A67+1</f>
+        <f t="shared" ref="A68:A109" si="6">A67+1</f>
         <v>66</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -2757,17 +2897,17 @@
         <v>26</v>
       </c>
       <c r="G68" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>res_rsaudcod_3508</v>
       </c>
       <c r="H68" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>def_sexo_feminino</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>67</v>
       </c>
       <c r="B69" s="1" t="s">
@@ -2780,17 +2920,17 @@
         <v>33</v>
       </c>
       <c r="G69" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>res_rsaudcod_3507</v>
       </c>
       <c r="H69" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>def_raca_cor_parda</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>68</v>
       </c>
       <c r="B70" s="1" t="s">
@@ -2803,17 +2943,17 @@
         <v>31</v>
       </c>
       <c r="G70" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>def_escol_nenhuma</v>
       </c>
       <c r="H70" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>def_raca_cor_ignorado</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>69</v>
       </c>
       <c r="B71" s="1" t="s">
@@ -2826,17 +2966,17 @@
         <v>93</v>
       </c>
       <c r="G71" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>def_escol_4_a_7_anos</v>
       </c>
       <c r="H71" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>res_csaudcod_35000</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>70</v>
       </c>
       <c r="B72" s="1" t="s">
@@ -2849,17 +2989,17 @@
         <v>66</v>
       </c>
       <c r="G72" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>dia_semana_obito_dom</v>
       </c>
       <c r="H72" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>res_msaudcod_3500</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>71</v>
       </c>
       <c r="B73" s="1" t="s">
@@ -2872,17 +3012,17 @@
         <v>68</v>
       </c>
       <c r="G73" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>def_loc_ocor_outros</v>
       </c>
       <c r="H73" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>res_rsaudcod_3500</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>72</v>
       </c>
       <c r="B74" s="1" t="s">
@@ -2895,17 +3035,17 @@
         <v>94</v>
       </c>
       <c r="G74" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>grande_grupo_ocup_trabalhadores_de_serviÃ§os_administrativos</v>
       </c>
       <c r="H74" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>res_csaudcod_35900</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>73</v>
       </c>
       <c r="B75" s="1" t="s">
@@ -2918,17 +3058,17 @@
         <v>67</v>
       </c>
       <c r="G75" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>res_rsaudcod_3511</v>
       </c>
       <c r="H75" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>res_msaudcod_3590</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>74</v>
       </c>
       <c r="B76" s="1" t="s">
@@ -2941,17 +3081,17 @@
         <v>53</v>
       </c>
       <c r="G76" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>dia_semana_nasc_sab</v>
       </c>
       <c r="H76" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>def_assist_med_ignorado</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>75</v>
       </c>
       <c r="B77" s="1" t="s">
@@ -2964,17 +3104,17 @@
         <v>40</v>
       </c>
       <c r="G77" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>def_raca_cor_indÃ­gena</v>
       </c>
       <c r="H77" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>def_escol_1_a_3_anos</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>76</v>
       </c>
       <c r="B78" s="1" t="s">
@@ -2987,17 +3127,17 @@
         <v>30</v>
       </c>
       <c r="G78" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>res_rsaudcod_3505</v>
       </c>
       <c r="H78" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>def_raca_cor_branca</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>77</v>
       </c>
       <c r="B79" s="1" t="s">
@@ -3010,17 +3150,17 @@
         <v>47</v>
       </c>
       <c r="G79" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>def_raca_cor_ignorado</v>
       </c>
       <c r="H79" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>def_loc_ocor_hospital</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>78</v>
       </c>
       <c r="B80" s="1" t="s">
@@ -3033,17 +3173,17 @@
         <v>61</v>
       </c>
       <c r="G80" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>res_rsaudcod_3514</v>
       </c>
       <c r="H80" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>def_necropsia_ignorado</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>79</v>
       </c>
       <c r="B81" s="1" t="s">
@@ -3056,17 +3196,17 @@
         <v>52</v>
       </c>
       <c r="G81" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>grande_grupo_ocup_trabalhadores_dos_serviÃ§os_vendedores_do_comÃ©rcio_em_lojas_e_mercados</v>
       </c>
       <c r="H81" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>def_assist_med_com_assistÃªncia</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>80</v>
       </c>
       <c r="B82" s="1" t="s">
@@ -3079,17 +3219,17 @@
         <v>56</v>
       </c>
       <c r="G82" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>def_cirurgia_nÃ£o</v>
       </c>
       <c r="H82" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>def_exame_nÃ£o</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>81</v>
       </c>
       <c r="B83" s="1" t="s">
@@ -3102,17 +3242,17 @@
         <v>36</v>
       </c>
       <c r="G83" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>def_necropsia_nÃ£o</v>
       </c>
       <c r="H83" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>def_est_civil_ignorado</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>82</v>
       </c>
       <c r="B84" s="1" t="s">
@@ -3125,17 +3265,17 @@
         <v>38</v>
       </c>
       <c r="G84" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>res_rsaudcod_3503</v>
       </c>
       <c r="H84" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>def_est_civil_solteiro</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>83</v>
       </c>
       <c r="B85" s="1" t="s">
@@ -3148,17 +3288,17 @@
         <v>63</v>
       </c>
       <c r="G85" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>res_rsaudcod_3524</v>
       </c>
       <c r="H85" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>def_necropsia_sim</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>84</v>
       </c>
       <c r="B86" s="1" t="s">
@@ -3171,17 +3311,17 @@
         <v>39</v>
       </c>
       <c r="G86" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>dia_semana_obito_sab</v>
       </c>
       <c r="H86" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>def_est_civil_viÃºvo</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>85</v>
       </c>
       <c r="B87" s="1" t="s">
@@ -3194,17 +3334,17 @@
         <v>10</v>
       </c>
       <c r="G87" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>def_exame_nÃ£o</v>
       </c>
       <c r="H87" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>ocor_area</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>86</v>
       </c>
       <c r="B88" s="1" t="s">
@@ -3217,17 +3357,17 @@
         <v>8</v>
       </c>
       <c r="G88" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>res_rsaudcod_3502</v>
       </c>
       <c r="H88" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>res_altitude</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>87</v>
       </c>
       <c r="B89" s="1" t="s">
@@ -3240,17 +3380,17 @@
         <v>9</v>
       </c>
       <c r="G89" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>dia_semana_obito_qui</v>
       </c>
       <c r="H89" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>res_area</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>88</v>
       </c>
       <c r="B90" s="1" t="s">
@@ -3263,17 +3403,17 @@
         <v>44</v>
       </c>
       <c r="G90" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>grande_grupo_ocup_trabalhadores_agropecuÃ¡rios_florestais_da_caÃ§a_e_pesca</v>
       </c>
       <c r="H90" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>def_escol_ignorado</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>89</v>
       </c>
       <c r="B91" s="1" t="s">
@@ -3286,17 +3426,17 @@
         <v>62</v>
       </c>
       <c r="G91" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>dia_semana_nasc_sex</v>
       </c>
       <c r="H91" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>def_necropsia_nÃ£o</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>90</v>
       </c>
       <c r="B92" s="1" t="s">
@@ -3309,17 +3449,17 @@
         <v>7</v>
       </c>
       <c r="G92" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>dia_semana_nasc_seg</v>
       </c>
       <c r="H92" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>res_longitude</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>91</v>
       </c>
       <c r="B93" s="1" t="s">
@@ -3332,17 +3472,17 @@
         <v>57</v>
       </c>
       <c r="G93" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>dia_semana_nasc_qua</v>
       </c>
       <c r="H93" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>def_exame_sim</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>92</v>
       </c>
       <c r="B94" s="1" t="s">
@@ -3355,17 +3495,17 @@
         <v>59</v>
       </c>
       <c r="G94" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>res_rsaudcod_3515</v>
       </c>
       <c r="H94" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>def_cirurgia_nÃ£o</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>93</v>
       </c>
       <c r="B95" s="1" t="s">
@@ -3378,17 +3518,17 @@
         <v>95</v>
       </c>
       <c r="G95" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>def_escol_1_a_3_anos</v>
       </c>
       <c r="H95" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>grande_grupo_ocup_forÃ§as_armadas_policiais_e_bombeiros_militares</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>94</v>
       </c>
       <c r="B96" s="1" t="s">
@@ -3401,17 +3541,17 @@
         <v>107</v>
       </c>
       <c r="G96" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>res_rsaudcod_3518</v>
       </c>
       <c r="H96" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>nivel_comp_ocup_nÃ£o_definido</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>95</v>
       </c>
       <c r="B97" s="1" t="s">
@@ -3424,17 +3564,17 @@
         <v>6</v>
       </c>
       <c r="G97" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>grande_grupo_ocup_profissionais_das_ciÃªncias_e_das_artes</v>
       </c>
       <c r="H97" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>res_latitude</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>96</v>
       </c>
       <c r="B98" s="1" t="s">
@@ -3447,17 +3587,17 @@
         <v>100</v>
       </c>
       <c r="G98" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>nivel_comp_ocup_nivel4</v>
       </c>
       <c r="H98" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>grande_grupo_ocup_trabalhadores_de_manutenÃ§Ã£o_e_reparaÃ§Ã£o</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>97</v>
       </c>
       <c r="B99" s="1" t="s">
@@ -3470,17 +3610,17 @@
         <v>58</v>
       </c>
       <c r="G99" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>res_rsaudcod_3510</v>
       </c>
       <c r="H99" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>def_cirurgia_ignorado</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>98</v>
       </c>
       <c r="B100" s="1" t="s">
@@ -3493,17 +3633,17 @@
         <v>55</v>
       </c>
       <c r="G100" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>grande_grupo_ocup_trabalhadores_de_manutenÃ§Ã£o_e_reparaÃ§Ã£o</v>
       </c>
       <c r="H100" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>def_exame_ignorado</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>99</v>
       </c>
       <c r="B101" s="1" t="s">
@@ -3516,17 +3656,17 @@
         <v>64</v>
       </c>
       <c r="G101" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>res_rsaudcod_3517</v>
       </c>
       <c r="H101" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>res_capital_n</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
       <c r="B102" s="1" t="s">
@@ -3539,17 +3679,17 @@
         <v>69</v>
       </c>
       <c r="G102" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>def_sexo_ignorado</v>
       </c>
       <c r="H102" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>res_rsaudcod_3501</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>101</v>
       </c>
       <c r="B103" s="1" t="s">
@@ -3562,17 +3702,17 @@
         <v>65</v>
       </c>
       <c r="G103" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>res_rsaudcod_3500</v>
       </c>
       <c r="H103" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>res_capital_s</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>102</v>
       </c>
       <c r="B104" s="1" t="s">
@@ -3585,17 +3725,17 @@
         <v>4</v>
       </c>
       <c r="G104" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>def_loc_ocor_via_pÃºblica</v>
       </c>
       <c r="H104" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>ano_nasc</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>103</v>
       </c>
       <c r="B105" s="1" t="s">
@@ -3608,17 +3748,17 @@
         <v>11</v>
       </c>
       <c r="G105" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>res_msaudcod_3590</v>
       </c>
       <c r="H105" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>idade_obito</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>104</v>
       </c>
       <c r="B106" s="1" t="s">
@@ -3631,17 +3771,17 @@
         <v>5</v>
       </c>
       <c r="G106" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>res_csaudcod_35900</v>
       </c>
       <c r="H106" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>idade_obito_anos</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>105</v>
       </c>
       <c r="B107" s="1" t="s">
@@ -3654,17 +3794,17 @@
         <v>3</v>
       </c>
       <c r="G107" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>res_csaudcod_35000</v>
       </c>
       <c r="H107" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>idade_obito_calculado</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>106</v>
       </c>
       <c r="B108" s="1" t="s">
@@ -3677,17 +3817,17 @@
         <v>104</v>
       </c>
       <c r="G108" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>def_loc_ocor_ignorado</v>
       </c>
       <c r="H108" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>nivel_comp_ocup_nivel2</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>107</v>
       </c>
       <c r="B109" s="1" t="s">
@@ -3700,11 +3840,11 @@
         <v>1</v>
       </c>
       <c r="G109" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>res_msaudcod_3500</v>
       </c>
       <c r="H109" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>ano_obito</v>
       </c>
     </row>

</xml_diff>